<commit_message>
changed code as suggest
</commit_message>
<xml_diff>
--- a/src/main/resources/excellRead.xlsx
+++ b/src/main/resources/excellRead.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="5460"/>
   </bookViews>
   <sheets>
     <sheet name="Planet Names" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,11 @@
     <sheet name="MoreValuesinTarget" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Routes!$B$1:$B$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Routes!$A$1:$D$46</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="83">
   <si>
     <t>Planet Node</t>
   </si>
@@ -279,11 +279,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,8 +375,36 @@
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -643,27 +671,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -671,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -679,7 +707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -687,7 +715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -695,7 +723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -703,7 +731,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -711,7 +739,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -719,7 +747,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -727,7 +755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -735,7 +763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -743,7 +771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -751,7 +779,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -759,7 +787,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -767,7 +795,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -775,7 +803,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -783,7 +811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -791,7 +819,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -799,7 +827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -807,7 +835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -815,7 +843,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -823,7 +851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -831,7 +859,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -839,7 +867,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -847,7 +875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -855,7 +883,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -863,7 +891,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -871,7 +899,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -879,7 +907,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -887,7 +915,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -895,7 +923,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -903,7 +931,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -911,7 +939,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -919,7 +947,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -927,7 +955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -935,7 +963,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -943,7 +971,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -951,7 +979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -959,7 +987,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -974,21 +1002,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -1002,7 +1030,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1016,7 +1044,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1030,7 +1058,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1044,7 +1072,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1057,8 +1085,17 @@
       <c r="D5" s="4">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="G5" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1071,8 +1108,17 @@
       <c r="D6" s="4">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="G6" s="4">
+        <v>2.44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1085,8 +1131,17 @@
       <c r="D7" s="4">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="G7" s="4">
+        <v>3.71</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1100,7 +1155,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1114,7 +1169,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1128,7 +1183,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1142,7 +1197,7 @@
         <v>8.09</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1156,7 +1211,7 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1170,7 +1225,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1184,7 +1239,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1198,7 +1253,7 @@
         <v>13.97</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1212,7 +1267,7 @@
         <v>14.78</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1226,7 +1281,7 @@
         <v>15.23</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1240,7 +1295,7 @@
         <v>10.43</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1254,7 +1309,7 @@
         <v>14.22</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1268,7 +1323,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1282,7 +1337,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1296,7 +1351,7 @@
         <v>12.34</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1310,7 +1365,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1324,7 +1379,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1338,7 +1393,7 @@
         <v>18.91</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1352,7 +1407,7 @@
         <v>22.04</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1366,7 +1421,7 @@
         <v>10.51</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1380,7 +1435,7 @@
         <v>23.61</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1394,7 +1449,7 @@
         <v>19.940000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1408,7 +1463,7 @@
         <v>9.31</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1422,7 +1477,7 @@
         <v>21.23</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1436,7 +1491,7 @@
         <v>25.96</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1450,7 +1505,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1464,7 +1519,7 @@
         <v>20.420000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1478,7 +1533,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1492,7 +1547,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1506,7 +1561,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1520,7 +1575,7 @@
         <v>23.13</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1534,7 +1589,7 @@
         <v>28.89</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1548,7 +1603,7 @@
         <v>10.64</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1562,7 +1617,7 @@
         <v>36.19</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1576,7 +1631,7 @@
         <v>36.479999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1590,7 +1645,7 @@
         <v>41.26</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1604,7 +1659,7 @@
         <v>42.07</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1618,7 +1673,7 @@
         <v>17.63</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1638,14 +1693,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -1653,7 +1708,7 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -1667,7 +1722,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1683,7 +1738,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1699,7 +1754,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1715,7 +1770,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1731,7 +1786,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1747,7 +1802,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1763,7 +1818,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1779,7 +1834,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1795,7 +1850,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1811,7 +1866,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1827,7 +1882,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1843,7 +1898,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1859,7 +1914,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1875,7 +1930,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1891,7 +1946,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1907,7 +1962,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1923,7 +1978,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1939,7 +1994,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1955,7 +2010,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1971,7 +2026,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1987,7 +2042,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2003,7 +2058,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2019,7 +2074,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2035,7 +2090,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2051,7 +2106,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2067,7 +2122,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2083,7 +2138,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2099,7 +2154,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2115,7 +2170,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2131,7 +2186,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2147,7 +2202,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2163,7 +2218,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2179,7 +2234,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2195,7 +2250,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2211,7 +2266,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2227,7 +2282,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2243,7 +2298,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2259,7 +2314,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2275,7 +2330,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2291,7 +2346,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2307,7 +2362,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2323,7 +2378,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2339,7 +2394,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2355,7 +2410,7 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2371,7 +2426,7 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2393,19 +2448,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -2422,7 +2477,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2439,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2456,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2473,7 +2528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2490,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2507,7 +2562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2527,7 +2582,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2544,7 +2599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2561,7 +2616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2578,7 +2633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2595,7 +2650,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2612,7 +2667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2629,7 +2684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2646,7 +2701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2663,7 +2718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2680,7 +2735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2697,7 +2752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2714,7 +2769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2748,7 +2803,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2765,7 +2820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2782,7 +2837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2799,7 +2854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2816,7 +2871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2833,7 +2888,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2850,7 +2905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2867,7 +2922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2884,7 +2939,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2901,7 +2956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2918,7 +2973,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2935,7 +2990,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2952,7 +3007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2963,7 +3018,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2974,7 +3029,7 @@
         <v>20.420000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2985,7 +3040,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2996,7 +3051,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3007,7 +3062,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3018,7 +3073,7 @@
         <v>23.13</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3026,7 +3081,7 @@
         <v>28.89</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3034,7 +3089,7 @@
         <v>10.64</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3042,7 +3097,7 @@
         <v>36.19</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3050,7 +3105,7 @@
         <v>36.479999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3058,7 +3113,7 @@
         <v>41.26</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3066,7 +3121,7 @@
         <v>42.07</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3074,7 +3129,7 @@
         <v>17.63</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>

</xml_diff>